<commit_message>
Remove unused Code ; Fix Api Endpoints HttpCodes
</commit_message>
<xml_diff>
--- a/project planning/API_Endpoints.xlsx
+++ b/project planning/API_Endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Resilio Sync\Daniel Schor\Studium\Module\Aktuell\WebApp\Projekt\Repo\webappproject23-24-devteam\project planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74560D0-B846-4684-863C-A222C7FF2E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136D9C9D-082B-423B-BA1B-A7C6B5DA9586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AEC6116-FBBD-4A6A-8287-4603E5F5CE05}"/>
   </bookViews>
@@ -156,16 +156,6 @@
 400 Bad Request</t>
   </si>
   <si>
-    <t>Location: /users/{userId}
-(keine zusätzlichen Header)
-(keine zusätzlichen Header)</t>
-  </si>
-  <si>
-    <t>Location: /events/{eventID}
-(keine zusätzlichen Header)
-(keine zusätzlichen Header)</t>
-  </si>
-  <si>
     <t>/events/remove/{userID}</t>
   </si>
   <si>
@@ -179,6 +169,16 @@
   <si>
     <t>201 Created
 400 Bad Request</t>
+  </si>
+  <si>
+    <t>Location: /events/{eventID}
+Location: /events
+(keine zusätzlichen Header)</t>
+  </si>
+  <si>
+    <t>Location: /users/{userId}
+Location: /users
+(keine zusätzlichen Header)</t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,12 +241,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor theme="6" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor theme="6" tint="0.79998168889431442"/>
       </patternFill>
@@ -464,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -535,9 +529,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -571,21 +562,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -602,6 +578,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -614,31 +593,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -653,83 +617,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1284,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9F2D08-239F-4D88-8E6A-1E4C636ABC07}">
   <dimension ref="B3:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,99 +1242,99 @@
     </row>
     <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
-      <c r="C4" s="68">
+      <c r="C4" s="6">
         <v>1</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="71" t="s">
+      <c r="F4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="73">
+      <c r="C5" s="11">
         <v>2</v>
       </c>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="76" t="s">
+      <c r="F5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="73">
+      <c r="C6" s="11">
         <v>3</v>
       </c>
-      <c r="D6" s="74" t="s">
+      <c r="D6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="76" t="s">
+      <c r="F6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="77" t="s">
-        <v>34</v>
+      <c r="G6" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="73">
+      <c r="C7" s="11">
         <v>4</v>
       </c>
-      <c r="D7" s="74" t="s">
+      <c r="D7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="76" t="s">
+      <c r="F7" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="77" t="s">
+      <c r="G7" s="18" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
-      <c r="C8" s="78">
+      <c r="C8" s="14">
         <v>5</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="82" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="91" t="s">
+      <c r="G8" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="91"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
     </row>
     <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -1467,37 +1386,37 @@
     </row>
     <row r="11" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
-      <c r="C11" s="73">
+      <c r="C11" s="11">
         <v>8</v>
       </c>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="76" t="s">
+      <c r="F11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="77" t="s">
-        <v>35</v>
+      <c r="G11" s="18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
-      <c r="C12" s="73">
+      <c r="C12" s="11">
         <v>9</v>
       </c>
-      <c r="D12" s="74" t="s">
+      <c r="D12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="75" t="s">
+      <c r="E12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="76" t="s">
+      <c r="F12" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="77" t="s">
+      <c r="G12" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1520,54 +1439,54 @@
       </c>
     </row>
     <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C14" s="68">
+      <c r="C14" s="6">
         <v>11</v>
       </c>
-      <c r="D14" s="74" t="s">
+      <c r="D14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="83" t="s">
+      <c r="E14" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="76" t="s">
+      <c r="F14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="77" t="s">
+      <c r="G14" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="73">
+      <c r="C15" s="11">
         <v>12</v>
       </c>
-      <c r="D15" s="74" t="s">
+      <c r="D15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="83" t="s">
+      <c r="E15" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="76" t="s">
+      <c r="F15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="77" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C16" s="73">
+      <c r="G15" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="C16" s="11">
         <v>13</v>
       </c>
-      <c r="D16" s="79" t="s">
+      <c r="D16" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="84" t="s">
+      <c r="E16" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="81" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="82" t="s">
-        <v>7</v>
+      <c r="F16" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1642,7 +1561,7 @@
         <v>12</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>13</v>
@@ -1727,7 +1646,7 @@
         <v>15</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>17</v>
@@ -1771,104 +1690,104 @@
       <c r="B30" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="26" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C31" s="28">
+      <c r="C31" s="27">
         <v>1</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="31" t="s">
+      <c r="F31" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C32" s="33">
+      <c r="C32" s="32">
         <v>2</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="36" t="s">
+      <c r="F32" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="36" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C33" s="38">
+      <c r="C33" s="32">
         <v>3</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="40" t="s">
+      <c r="E33" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="41" t="s">
+      <c r="F33" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="G33" s="42" t="s">
-        <v>34</v>
+      <c r="G33" s="36" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C34" s="33">
+      <c r="C34" s="32">
         <v>4</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="36" t="s">
+      <c r="F34" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="G34" s="37" t="s">
+      <c r="G34" s="36" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C35" s="43">
+      <c r="C35" s="37">
         <v>5</v>
       </c>
-      <c r="D35" s="44" t="s">
+      <c r="D35" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="45" t="s">
+      <c r="E35" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="46" t="s">
+      <c r="F35" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="47" t="s">
+      <c r="G35" s="41" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1876,19 +1795,19 @@
       <c r="B37" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E37" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G37" s="27" t="s">
+      <c r="G37" s="26" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1896,67 +1815,67 @@
       <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F38" s="31" t="s">
+      <c r="F38" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="32" t="s">
+      <c r="G38" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C39" s="53">
+      <c r="C39" s="43">
         <v>2</v>
       </c>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="55" t="s">
+      <c r="E39" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="56" t="s">
+      <c r="F39" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="57" t="s">
+      <c r="G39" s="47" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C40" s="25">
+      <c r="C40" s="11">
         <v>3</v>
       </c>
-      <c r="D40" s="49" t="s">
+      <c r="D40" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="50" t="s">
+      <c r="E40" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="51" t="s">
+      <c r="F40" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="G40" s="52" t="s">
-        <v>35</v>
+      <c r="G40" s="47" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C41" s="53">
+      <c r="C41" s="43">
         <v>4</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="35" t="s">
+      <c r="E41" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="36" t="s">
+      <c r="F41" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="G41" s="37" t="s">
+      <c r="G41" s="36" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1964,67 +1883,67 @@
       <c r="C42" s="11">
         <v>5</v>
       </c>
-      <c r="D42" s="58" t="s">
+      <c r="D42" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="59" t="s">
+      <c r="E42" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="60" t="s">
+      <c r="F42" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="61" t="s">
+      <c r="G42" s="51" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C43" s="89">
+      <c r="C43" s="62">
         <v>6</v>
       </c>
-      <c r="D43" s="86" t="s">
+      <c r="D43" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="90" t="s">
+      <c r="E43" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="F43" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="F43" s="87" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="88" t="s">
-        <v>37</v>
+      <c r="G43" s="61" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C44" s="11">
         <v>7</v>
       </c>
-      <c r="D44" s="62" t="s">
+      <c r="D44" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="63" t="s">
+      <c r="E44" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="F44" s="64" t="s">
+      <c r="F44" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="65" t="s">
+      <c r="G44" s="55" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C45" s="53">
+      <c r="C45" s="43">
         <v>8</v>
       </c>
-      <c r="D45" s="54" t="s">
+      <c r="D45" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="66" t="s">
+      <c r="E45" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="F45" s="56" t="s">
+      <c r="F45" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G45" s="85" t="s">
+      <c r="G45" s="58" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2032,16 +1951,16 @@
       <c r="C46" s="14">
         <v>9</v>
       </c>
-      <c r="D46" s="44" t="s">
+      <c r="D46" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E46" s="67" t="s">
+      <c r="E46" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="F46" s="46" t="s">
+      <c r="F46" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="G46" s="47" t="s">
+      <c r="G46" s="41" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove unused Code ; Add API Endpoint: /events/{eventID}/participants
</commit_message>
<xml_diff>
--- a/project planning/API_Endpoints.xlsx
+++ b/project planning/API_Endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Resilio Sync\Daniel Schor\Studium\Module\Aktuell\WebApp\Projekt\Repo\webappproject23-24-devteam\project planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136D9C9D-082B-423B-BA1B-A7C6B5DA9586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60306148-16E2-447C-A992-6A95CACF6848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AEC6116-FBBD-4A6A-8287-4603E5F5CE05}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="40">
   <si>
     <t>No.</t>
   </si>
@@ -159,14 +159,6 @@
     <t>/events/remove/{userID}</t>
   </si>
   <si>
-    <t xml:space="preserve">(keine zusätzlichen Header)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">204 No Content
-</t>
-  </si>
-  <si>
     <t>201 Created
 400 Bad Request</t>
   </si>
@@ -179,6 +171,14 @@
     <t>Location: /users/{userId}
 Location: /users
 (keine zusätzlichen Header)</t>
+  </si>
+  <si>
+    <t>/events/{eventID}/participants</t>
+  </si>
+  <si>
+    <t>200 OK
+204 No Content
+404 Not Found</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -626,29 +626,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -877,8 +862,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}" name="Tabelle2" displayName="Tabelle2" ref="C3:G16" totalsRowShown="0" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="C3:G16" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}" name="Tabelle2" displayName="Tabelle2" ref="C3:G17" totalsRowShown="0" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="C3:G17" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DC6E2D57-066A-454A-9442-01C57A7F31A0}" name="No." dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{95550AC8-0C27-4875-A6C7-CCCAFB9DFD52}" name="HTTP-Methode" dataDxfId="10"/>
@@ -891,8 +876,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}" name="Tabelle22" displayName="Tabelle22" ref="C18:G28" totalsRowShown="0" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="C18:G28" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}" name="Tabelle22" displayName="Tabelle22" ref="C19:G29" totalsRowShown="0" dataDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="C19:G29" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{311040A3-5AC1-4F93-A9EC-561F780EBAA0}" name="No." dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{21F7FAD3-B3CC-40CC-ACB8-7628049521CE}" name="HTTP-Methode" dataDxfId="3"/>
@@ -1201,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9F2D08-239F-4D88-8E6A-1E4C636ABC07}">
-  <dimension ref="B3:L46"/>
+  <dimension ref="B3:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,7 +1276,7 @@
         <v>33</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="45" x14ac:dyDescent="0.25">
@@ -1314,7 +1299,7 @@
     </row>
     <row r="8" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
-      <c r="C8" s="14">
+      <c r="C8" s="11">
         <v>5</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -1329,12 +1314,12 @@
       <c r="G8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
     </row>
     <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -1389,17 +1374,17 @@
       <c r="C11" s="11">
         <v>8</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="18" t="s">
+      <c r="D11" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="34" t="s">
         <v>38</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="36" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="45" x14ac:dyDescent="0.25">
@@ -1408,50 +1393,51 @@
         <v>9</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="11">
         <v>10</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="D13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F13" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G13" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="14">
-        <v>10</v>
-      </c>
-      <c r="D13" s="15" t="s">
+    <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="14">
         <v>11</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="D14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F14" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C14" s="6">
-        <v>11</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="24" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1462,8 +1448,8 @@
       <c r="D15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="65" t="s">
-        <v>30</v>
+      <c r="E15" s="59" t="s">
+        <v>29</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>8</v>
@@ -1472,164 +1458,164 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="11">
         <v>13</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="66" t="s">
+      <c r="E16" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="14">
+        <v>14</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G17" s="24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C19" s="6">
+    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="6">
         <v>1</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F20" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C20" s="11">
-        <v>2</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="11">
+        <v>2</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="11">
         <v>3</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E22" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="18" t="s">
+      <c r="F22" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C22" s="11">
+    <row r="23" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C23" s="11">
         <v>4</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D23" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F23" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G23" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C23" s="14">
+    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="14">
         <v>5</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D24" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E24" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F24" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="11">
-        <v>6</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="18" t="s">
+      <c r="G24" s="24" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>7</v>
@@ -1637,330 +1623,347 @@
     </row>
     <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="11">
+        <v>7</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="G26" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="11">
+        <v>8</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E27" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" s="18" t="s">
+      <c r="F27" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C27" s="11">
+    <row r="28" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C28" s="11">
         <v>9</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E28" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F28" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G28" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C28" s="14">
+    <row r="29" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="14">
         <v>10</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E29" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F29" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="G29" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C31" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D31" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E31" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="25" t="s">
+      <c r="F31" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G30" s="26" t="s">
+      <c r="G31" s="26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C31" s="27">
+    <row r="32" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C32" s="27">
         <v>1</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D32" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="29" t="s">
+      <c r="E32" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="30" t="s">
+      <c r="F32" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C32" s="32">
+      <c r="G32" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="32">
         <v>2</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D33" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E33" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="35" t="s">
+      <c r="F33" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C33" s="32">
-        <v>3</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="35" t="s">
-        <v>33</v>
-      </c>
       <c r="G33" s="36" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C34" s="32">
+        <v>3</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C35" s="32">
         <v>4</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D35" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E35" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="35" t="s">
+      <c r="F35" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="G34" s="36" t="s">
+      <c r="G35" s="36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C35" s="37">
+    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="37">
         <v>5</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D36" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="39" t="s">
+      <c r="E36" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="40" t="s">
+      <c r="F36" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="G36" s="41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C38" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D38" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E38" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="25" t="s">
+      <c r="F38" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G37" s="26" t="s">
+      <c r="G38" s="26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C38" s="6">
+    <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C39" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D39" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="29" t="s">
+      <c r="E39" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F38" s="30" t="s">
+      <c r="F39" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C39" s="43">
+      <c r="G39" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C40" s="43">
         <v>2</v>
       </c>
-      <c r="D39" s="44" t="s">
+      <c r="D40" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="45" t="s">
+      <c r="E40" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="46" t="s">
+      <c r="F40" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C40" s="11">
+      <c r="G40" s="47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C41" s="11">
         <v>3</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D41" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="45" t="s">
+      <c r="E41" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="46" t="s">
+      <c r="F41" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="G40" s="47" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C41" s="43">
+      <c r="G41" s="47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C42" s="43">
         <v>4</v>
       </c>
-      <c r="D41" s="33" t="s">
+      <c r="D42" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E42" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F42" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="G41" s="36" t="s">
+      <c r="G42" s="36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C42" s="11">
+    <row r="43" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C43" s="14">
         <v>5</v>
       </c>
-      <c r="D42" s="48" t="s">
+      <c r="D43" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="49" t="s">
+      <c r="E43" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="50" t="s">
+      <c r="F43" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="51" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C43" s="62">
+      <c r="G43" s="51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C44" s="43">
         <v>6</v>
       </c>
-      <c r="D43" s="59" t="s">
+      <c r="D44" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="63" t="s">
+      <c r="E44" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="F43" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="G43" s="61" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C44" s="11">
-        <v>7</v>
-      </c>
-      <c r="D44" s="52" t="s">
+      <c r="F44" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C45" s="11">
+        <v>7</v>
+      </c>
+      <c r="D45" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="53" t="s">
+      <c r="E45" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="F44" s="54" t="s">
+      <c r="F45" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="55" t="s">
+      <c r="G45" s="55" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C45" s="43">
+    <row r="46" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C46" s="43">
         <v>8</v>
       </c>
-      <c r="D45" s="44" t="s">
+      <c r="D46" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="56" t="s">
+      <c r="E46" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="F45" s="46" t="s">
+      <c r="F46" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G45" s="58" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C46" s="14">
+      <c r="G46" s="58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C47" s="14">
         <v>9</v>
       </c>
-      <c r="D46" s="38" t="s">
+      <c r="D47" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E46" s="57" t="s">
+      <c r="E47" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="F46" s="40" t="s">
+      <c r="F47" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="G46" s="41" t="s">
+      <c r="G47" s="41" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update API logging messages
</commit_message>
<xml_diff>
--- a/project planning/API_Endpoints.xlsx
+++ b/project planning/API_Endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Resilio Sync\Daniel Schor\Studium\Module\Aktuell\WebApp\Projekt\Repo\webappproject23-24-devteam\project planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Daniel Schor\Studium\Module\Aktuell\WebApp\Projekt\Repo\webappproject23-24-devteam\project planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60306148-16E2-447C-A992-6A95CACF6848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D848C4-B6F2-4588-8F48-17CE3E0B35A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AEC6116-FBBD-4A6A-8287-4603E5F5CE05}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13996" xr2:uid="{9AEC6116-FBBD-4A6A-8287-4603E5F5CE05}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -246,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -454,11 +454,188 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -635,11 +812,275 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="17">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -744,101 +1185,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -862,28 +1208,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}" name="Tabelle2" displayName="Tabelle2" ref="C3:G17" totalsRowShown="0" dataDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}" name="Tabelle2" displayName="Tabelle2" ref="C3:G17" totalsRowShown="0" headerRowDxfId="0" dataDxfId="16" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
   <autoFilter ref="C3:G17" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DC6E2D57-066A-454A-9442-01C57A7F31A0}" name="No." dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{95550AC8-0C27-4875-A6C7-CCCAFB9DFD52}" name="HTTP-Methode" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{0C62839A-F579-4042-866B-5EF0B9216FA1}" name="URl" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{A0DA9802-9B37-436F-B225-D48AA35CC625}" name="HTTP-Statuscode(s)" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{95E14EF1-88FA-4E26-BF8D-8695B027DCF1}" name="HTTP Header" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{DC6E2D57-066A-454A-9442-01C57A7F31A0}" name="No." dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{95550AC8-0C27-4875-A6C7-CCCAFB9DFD52}" name="HTTP-Methode" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{0C62839A-F579-4042-866B-5EF0B9216FA1}" name="URl" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A0DA9802-9B37-436F-B225-D48AA35CC625}" name="HTTP-Statuscode(s)" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{95E14EF1-88FA-4E26-BF8D-8695B027DCF1}" name="HTTP Header" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}" name="Tabelle22" displayName="Tabelle22" ref="C19:G29" totalsRowShown="0" dataDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}" name="Tabelle22" displayName="Tabelle22" ref="C19:G29" totalsRowShown="0" dataDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="C19:G29" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{311040A3-5AC1-4F93-A9EC-561F780EBAA0}" name="No." dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{21F7FAD3-B3CC-40CC-ACB8-7628049521CE}" name="HTTP-Methode" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{3B012289-4A30-4C7E-B7C5-17C1A8578C6F}" name="URl" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{069F9D91-DC39-4594-86BC-C0E078086CAF}" name="HTTP-Statuscode(s)" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{9C55A180-DB51-456F-B6B3-E017B0238133}" name="HTTP Header" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{311040A3-5AC1-4F93-A9EC-561F780EBAA0}" name="No." dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{21F7FAD3-B3CC-40CC-ACB8-7628049521CE}" name="HTTP-Methode" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{3B012289-4A30-4C7E-B7C5-17C1A8578C6F}" name="URl" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{069F9D91-DC39-4594-86BC-C0E078086CAF}" name="HTTP-Statuscode(s)" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{9C55A180-DB51-456F-B6B3-E017B0238133}" name="HTTP Header" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1188,130 +1534,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9F2D08-239F-4D88-8E6A-1E4C636ABC07}">
   <dimension ref="B3:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" customWidth="1"/>
-    <col min="7" max="7" width="45.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.1328125" customWidth="1"/>
+    <col min="3" max="3" width="11.3984375" customWidth="1"/>
+    <col min="4" max="4" width="15.265625" customWidth="1"/>
+    <col min="5" max="5" width="39.59765625" customWidth="1"/>
+    <col min="6" max="6" width="29.1328125" customWidth="1"/>
+    <col min="7" max="7" width="45.1328125" customWidth="1"/>
+    <col min="9" max="9" width="13.1328125" customWidth="1"/>
+    <col min="10" max="10" width="14.3984375" customWidth="1"/>
+    <col min="11" max="11" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="62" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
-      <c r="C4" s="6">
+      <c r="C4" s="77">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B5" s="2"/>
-      <c r="C5" s="11">
+      <c r="C5" s="82">
         <v>2</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5" s="83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B6" s="2"/>
-      <c r="C6" s="11">
+      <c r="C6" s="82">
         <v>3</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="83" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B7" s="2"/>
-      <c r="C7" s="11">
+      <c r="C7" s="82">
         <v>4</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="83" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="2"/>
-      <c r="C8" s="11">
+      <c r="C8" s="84">
         <v>5</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="88" t="s">
         <v>7</v>
       </c>
       <c r="I8" s="61" t="s">
@@ -1321,21 +1667,21 @@
       <c r="K8" s="61"/>
       <c r="L8" s="61"/>
     </row>
-    <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B9" s="2"/>
-      <c r="C9" s="6">
+      <c r="C9" s="77">
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="81" t="s">
         <v>7</v>
       </c>
       <c r="I9" s="19" t="s">
@@ -1351,155 +1697,155 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B10" s="2"/>
-      <c r="C10" s="11">
-        <v>7</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="82">
+        <v>7</v>
+      </c>
+      <c r="D10" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="G10" s="83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B11" s="2"/>
-      <c r="C11" s="11">
+      <c r="C11" s="82">
         <v>8</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="83" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B12" s="2"/>
-      <c r="C12" s="11">
+      <c r="C12" s="82">
         <v>9</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="83" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B13" s="2"/>
-      <c r="C13" s="11">
+      <c r="C13" s="82">
         <v>10</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="83" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="2"/>
-      <c r="C14" s="14">
+      <c r="C14" s="84">
         <v>11</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="11">
+      <c r="G14" s="88" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C15" s="74">
         <v>12</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C16" s="11">
+      <c r="G15" s="76" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C16" s="64">
         <v>13</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C17" s="14">
+      <c r="G16" s="67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="C17" s="69">
         <v>14</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="72" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="4"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>25</v>
       </c>
@@ -1519,7 +1865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C20" s="6">
         <v>1</v>
       </c>
@@ -1536,7 +1882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C21" s="11">
         <v>2</v>
       </c>
@@ -1553,7 +1899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C22" s="11">
         <v>3</v>
       </c>
@@ -1570,7 +1916,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="C23" s="11">
         <v>4</v>
       </c>
@@ -1587,7 +1933,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C24" s="14">
         <v>5</v>
       </c>
@@ -1604,7 +1950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C25" s="11">
         <v>6</v>
       </c>
@@ -1621,7 +1967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C26" s="11">
         <v>7</v>
       </c>
@@ -1638,7 +1984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C27" s="11">
         <v>8</v>
       </c>
@@ -1655,7 +2001,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="C28" s="11">
         <v>9</v>
       </c>
@@ -1672,7 +2018,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C29" s="14">
         <v>10</v>
       </c>
@@ -1689,7 +2035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>26</v>
       </c>
@@ -1709,7 +2055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C32" s="27">
         <v>1</v>
       </c>
@@ -1726,7 +2072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C33" s="32">
         <v>2</v>
       </c>
@@ -1743,7 +2089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="C34" s="32">
         <v>3</v>
       </c>
@@ -1760,7 +2106,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="C35" s="32">
         <v>4</v>
       </c>
@@ -1777,7 +2123,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C36" s="37">
         <v>5</v>
       </c>
@@ -1794,7 +2140,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>27</v>
       </c>
@@ -1814,7 +2160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C39" s="6">
         <v>1</v>
       </c>
@@ -1831,7 +2177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C40" s="43">
         <v>2</v>
       </c>
@@ -1848,7 +2194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="C41" s="11">
         <v>3</v>
       </c>
@@ -1865,7 +2211,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="C42" s="43">
         <v>4</v>
       </c>
@@ -1882,7 +2228,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C43" s="14">
         <v>5</v>
       </c>
@@ -1899,7 +2245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C44" s="43">
         <v>6</v>
       </c>
@@ -1916,7 +2262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="C45" s="11">
         <v>7</v>
       </c>
@@ -1933,7 +2279,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C46" s="43">
         <v>8</v>
       </c>
@@ -1950,7 +2296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="C47" s="14">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Add API PATCH user/event Endpoint
</commit_message>
<xml_diff>
--- a/project planning/API_Endpoints.xlsx
+++ b/project planning/API_Endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Daniel Schor\Studium\Module\Aktuell\WebApp\Projekt\Repo\webappproject23-24-devteam\project planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Resilio Sync\Daniel Schor\Studium\Module\Aktuell\WebApp\Projekt\Repo\webappproject23-24-devteam\project planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D848C4-B6F2-4588-8F48-17CE3E0B35A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC306BA-8B37-4E15-9B35-69ABAEF54D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13996" xr2:uid="{9AEC6116-FBBD-4A6A-8287-4603E5F5CE05}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AEC6116-FBBD-4A6A-8287-4603E5F5CE05}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="43">
   <si>
     <t>No.</t>
   </si>
@@ -179,6 +179,15 @@
     <t>200 OK
 204 No Content
 404 Not Found</t>
+  </si>
+  <si>
+    <t>/users/update/{userID}</t>
+  </si>
+  <si>
+    <t>/events/update/{eventID}</t>
+  </si>
+  <si>
+    <t>PATCH</t>
   </si>
 </sst>
 </file>
@@ -246,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -455,37 +464,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -499,11 +477,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -512,7 +492,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -530,7 +510,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -542,13 +522,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -566,7 +561,22 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -581,7 +591,33 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -593,7 +629,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -608,7 +644,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -623,7 +659,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -635,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -709,9 +745,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -724,9 +757,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -738,9 +768,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -809,84 +836,63 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -902,6 +908,40 @@
         </right>
         <top/>
         <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -1022,63 +1062,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1185,6 +1168,29 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1208,28 +1214,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}" name="Tabelle2" displayName="Tabelle2" ref="C3:G17" totalsRowShown="0" headerRowDxfId="0" dataDxfId="16" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="C3:G17" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}" name="Tabelle2" displayName="Tabelle2" ref="C3:G19" totalsRowShown="0" headerRowDxfId="0" dataDxfId="16" headerRowBorderDxfId="1" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="C3:G19" xr:uid="{F9B5A248-0A50-40EB-B955-9C63445F86B6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DC6E2D57-066A-454A-9442-01C57A7F31A0}" name="No." dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{95550AC8-0C27-4875-A6C7-CCCAFB9DFD52}" name="HTTP-Methode" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{0C62839A-F579-4042-866B-5EF0B9216FA1}" name="URl" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{A0DA9802-9B37-436F-B225-D48AA35CC625}" name="HTTP-Statuscode(s)" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{95E14EF1-88FA-4E26-BF8D-8695B027DCF1}" name="HTTP Header" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{DC6E2D57-066A-454A-9442-01C57A7F31A0}" name="No." dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{95550AC8-0C27-4875-A6C7-CCCAFB9DFD52}" name="HTTP-Methode" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{0C62839A-F579-4042-866B-5EF0B9216FA1}" name="URl" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{A0DA9802-9B37-436F-B225-D48AA35CC625}" name="HTTP-Statuscode(s)" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{95E14EF1-88FA-4E26-BF8D-8695B027DCF1}" name="HTTP Header" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}" name="Tabelle22" displayName="Tabelle22" ref="C19:G29" totalsRowShown="0" dataDxfId="15" tableBorderDxfId="14">
-  <autoFilter ref="C19:G29" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}" name="Tabelle22" displayName="Tabelle22" ref="C21:G31" totalsRowShown="0" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="C21:G31" xr:uid="{306496EB-F9C2-4FF8-8AFD-A8CEB1C5144A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{311040A3-5AC1-4F93-A9EC-561F780EBAA0}" name="No." dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{21F7FAD3-B3CC-40CC-ACB8-7628049521CE}" name="HTTP-Methode" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{3B012289-4A30-4C7E-B7C5-17C1A8578C6F}" name="URl" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{069F9D91-DC39-4594-86BC-C0E078086CAF}" name="HTTP-Statuscode(s)" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{9C55A180-DB51-456F-B6B3-E017B0238133}" name="HTTP Header" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{311040A3-5AC1-4F93-A9EC-561F780EBAA0}" name="No." dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{21F7FAD3-B3CC-40CC-ACB8-7628049521CE}" name="HTTP-Methode" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{3B012289-4A30-4C7E-B7C5-17C1A8578C6F}" name="URl" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{069F9D91-DC39-4594-86BC-C0E078086CAF}" name="HTTP-Statuscode(s)" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{9C55A180-DB51-456F-B6B3-E017B0238133}" name="HTTP Header" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1532,790 +1538,861 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9F2D08-239F-4D88-8E6A-1E4C636ABC07}">
-  <dimension ref="B3:L47"/>
+  <dimension ref="B2:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.1328125" customWidth="1"/>
-    <col min="3" max="3" width="11.3984375" customWidth="1"/>
-    <col min="4" max="4" width="15.265625" customWidth="1"/>
-    <col min="5" max="5" width="39.59765625" customWidth="1"/>
-    <col min="6" max="6" width="29.1328125" customWidth="1"/>
-    <col min="7" max="7" width="45.1328125" customWidth="1"/>
-    <col min="9" max="9" width="13.1328125" customWidth="1"/>
-    <col min="10" max="10" width="14.3984375" customWidth="1"/>
-    <col min="11" max="11" width="13.59765625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="7" max="7" width="45.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="78" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
-      <c r="C4" s="77">
+      <c r="C4" s="60">
         <v>1</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="79" t="s">
+      <c r="E4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="80" t="s">
+      <c r="F4" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="81" t="s">
+      <c r="G4" s="63" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="82">
+      <c r="C5" s="64">
         <v>2</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="58" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="83" t="s">
+      <c r="G5" s="65" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="82">
+      <c r="C6" s="64">
         <v>3</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="58" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="83" t="s">
+      <c r="G6" s="65" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="C7" s="82">
+      <c r="C7" s="64">
         <v>4</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="58" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="83" t="s">
+      <c r="G7" s="65" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
-      <c r="C8" s="84">
+      <c r="C8" s="64">
         <v>5</v>
       </c>
-      <c r="D8" s="85" t="s">
+      <c r="D8" s="73" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="66">
+        <v>6</v>
+      </c>
+      <c r="D9" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="86" t="s">
+      <c r="E9" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="87" t="s">
+      <c r="F9" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="88" t="s">
+      <c r="G9" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="61" t="s">
+      <c r="I9" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-    </row>
-    <row r="9" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B9" s="2"/>
-      <c r="C9" s="77">
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
+    </row>
+    <row r="10" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="60">
+        <v>7</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="78" t="s">
+      <c r="G10" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="64">
+        <v>8</v>
+      </c>
+      <c r="D11" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="79" t="s">
+      <c r="E11" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="64">
+        <v>9</v>
+      </c>
+      <c r="D12" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="64">
+        <v>10</v>
+      </c>
+      <c r="D13" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="80" t="s">
+      <c r="F13" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="65" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="64">
+        <v>11</v>
+      </c>
+      <c r="D14" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="64">
+        <v>12</v>
+      </c>
+      <c r="D15" s="73" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="66">
+        <v>13</v>
+      </c>
+      <c r="D16" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="69" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="14">
+        <v>14</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="75">
+        <v>15</v>
+      </c>
+      <c r="D18" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C19" s="75">
+        <v>16</v>
+      </c>
+      <c r="D19" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="81" t="s">
+      <c r="G22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B10" s="2"/>
-      <c r="C10" s="82">
-        <v>7</v>
-      </c>
-      <c r="D10" s="65" t="s">
+    </row>
+    <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C23" s="11">
+        <v>2</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="E10" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="83" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B11" s="2"/>
-      <c r="C11" s="82">
-        <v>8</v>
-      </c>
-      <c r="D11" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="83" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B12" s="2"/>
-      <c r="C12" s="82">
-        <v>9</v>
-      </c>
-      <c r="D12" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="83" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B13" s="2"/>
-      <c r="C13" s="82">
-        <v>10</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="83" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="2"/>
-      <c r="C14" s="84">
-        <v>11</v>
-      </c>
-      <c r="D14" s="85" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="88" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C15" s="74">
-        <v>12</v>
-      </c>
-      <c r="D15" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="60" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="76" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C16" s="64">
-        <v>13</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="67" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="C17" s="69">
-        <v>14</v>
-      </c>
-      <c r="D17" s="70" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="71" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="72" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B18" s="4"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C20" s="6">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C21" s="11">
-        <v>2</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C22" s="11">
-        <v>3</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="C23" s="11">
-        <v>4</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>10</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="11">
+        <v>3</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C25" s="11">
+        <v>4</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G25" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C24" s="14">
+    <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="14">
         <v>5</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D26" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E26" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="F26" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="24" t="s">
+      <c r="G26" s="24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C25" s="11">
+    <row r="27" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="11">
         <v>6</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D27" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C26" s="11">
-        <v>7</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C27" s="11">
-        <v>8</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C28" s="11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="11">
+        <v>8</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C30" s="11">
+        <v>9</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="G30" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C29" s="14">
+    <row r="31" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C31" s="14">
         <v>10</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D31" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E31" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F31" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G31" s="24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B31" t="s">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C33" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D33" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E33" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="25" t="s">
+      <c r="F33" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="26" t="s">
+      <c r="G33" s="26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C32" s="27">
+    <row r="34" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C34" s="6">
         <v>1</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D34" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E34" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="30" t="s">
+      <c r="F34" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G34" s="30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C33" s="32">
+    <row r="35" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C35" s="11">
         <v>2</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D35" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E35" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="35" t="s">
+      <c r="F35" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="36" t="s">
+      <c r="G35" s="34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="C34" s="32">
+    <row r="36" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C36" s="11">
         <v>3</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D36" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E36" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="35" t="s">
+      <c r="F36" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G34" s="36" t="s">
+      <c r="G36" s="34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="C35" s="32">
+    <row r="37" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C37" s="11">
         <v>4</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D37" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="34" t="s">
+      <c r="E37" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="35" t="s">
+      <c r="F37" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G35" s="36" t="s">
+      <c r="G37" s="34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C36" s="37">
+    <row r="38" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C38" s="11">
         <v>5</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D38" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C39" s="14">
+        <v>6</v>
+      </c>
+      <c r="D39" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="39" t="s">
+      <c r="E39" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="40" t="s">
+      <c r="F39" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="41" t="s">
+      <c r="G39" s="38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B38" t="s">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C41" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="25" t="s">
+      <c r="D41" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E41" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="25" t="s">
+      <c r="F41" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="26" t="s">
+      <c r="G41" s="26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C39" s="6">
+    <row r="42" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C42" s="6">
         <v>1</v>
       </c>
-      <c r="D39" s="28" t="s">
+      <c r="D42" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="29" t="s">
+      <c r="E42" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F39" s="30" t="s">
+      <c r="F42" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G39" s="31" t="s">
+      <c r="G42" s="30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C40" s="43">
+    <row r="43" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C43" s="40">
         <v>2</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D43" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="45" t="s">
+      <c r="E43" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="46" t="s">
+      <c r="F43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="47" t="s">
+      <c r="G43" s="44" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="C41" s="11">
+    <row r="44" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C44" s="11">
         <v>3</v>
       </c>
-      <c r="D41" s="44" t="s">
+      <c r="D44" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="45" t="s">
+      <c r="E44" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="F41" s="46" t="s">
+      <c r="F44" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="G41" s="47" t="s">
+      <c r="G44" s="44" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="C42" s="43">
+    <row r="45" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C45" s="40">
         <v>4</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D45" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="34" t="s">
+      <c r="E45" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="35" t="s">
+      <c r="F45" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G42" s="36" t="s">
+      <c r="G45" s="34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C43" s="14">
+    <row r="46" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C46" s="11">
         <v>5</v>
       </c>
-      <c r="D43" s="48" t="s">
+      <c r="D46" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C47" s="71">
+        <v>6</v>
+      </c>
+      <c r="D47" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="49" t="s">
+      <c r="E47" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="50" t="s">
+      <c r="F47" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G43" s="51" t="s">
+      <c r="G47" s="48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C44" s="43">
-        <v>6</v>
-      </c>
-      <c r="D44" s="12" t="s">
+    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C48" s="11">
+        <v>7</v>
+      </c>
+      <c r="D48" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="59" t="s">
+      <c r="E48" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="F48" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G44" s="18" t="s">
+      <c r="G48" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="C45" s="11">
+    <row r="49" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C49" s="40">
+        <v>8</v>
+      </c>
+      <c r="D49" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="G49" s="52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C50" s="11">
+        <v>9</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="F50" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="52" t="s">
+    </row>
+    <row r="51" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C51" s="71">
         <v>10</v>
       </c>
-      <c r="E45" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="F45" s="54" t="s">
+      <c r="D51" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="G45" s="55" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="C46" s="43">
-        <v>8</v>
-      </c>
-      <c r="D46" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="F46" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" s="58" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="C47" s="14">
-        <v>9</v>
-      </c>
-      <c r="D47" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="F47" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47" s="41" t="s">
+      <c r="G51" s="38" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>